<commit_message>
Finalized HMI to first integrated and working version
</commit_message>
<xml_diff>
--- a/HMI/Datasheets/SAMC21/SAMC21_Pinout.xlsx
+++ b/HMI/Datasheets/SAMC21/SAMC21_Pinout.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domin\Desktop\_work\X2City\HMI\Datasheets\SAMC21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5E9C10-DBFF-4F8C-8548-6C6C5083BF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A171CF-22AC-4FBA-884B-2796402053FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{B9B784E2-40E7-46A1-B6A9-A010A1749725}"/>
   </bookViews>
@@ -21,12 +21,20 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="202">
   <si>
     <t>PORT_PA11</t>
   </si>
@@ -608,13 +616,37 @@
   </si>
   <si>
     <t>SPI-&gt;CS ADS</t>
+  </si>
+  <si>
+    <t>CanCom L</t>
+  </si>
+  <si>
+    <t>CanCom H</t>
+  </si>
+  <si>
+    <t>SSD1327-&gt;SDA</t>
+  </si>
+  <si>
+    <t>SSD1327-&gt;SCL</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>IO/Light</t>
+  </si>
+  <si>
+    <t>Hall-&gt;GND</t>
+  </si>
+  <si>
+    <t>Hall-&gt;SIG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -630,8 +662,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -665,6 +704,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -761,7 +824,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -798,6 +861,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -822,13 +895,13 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>10182</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>104446</xdr:rowOff>
+      <xdr:rowOff>97877</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>1586733</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>63103</xdr:rowOff>
+      <xdr:rowOff>69672</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -858,7 +931,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9587734" y="492015"/>
+          <a:off x="9587734" y="505153"/>
           <a:ext cx="2338551" cy="3243140"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1244,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABC464E6-459F-468A-901F-AD48611239EA}">
-  <dimension ref="A2:AD18"/>
+  <dimension ref="A1:AD29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1269,7 +1342,7 @@
     <col min="17" max="17" width="16.5703125" customWidth="1"/>
     <col min="18" max="18" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7" bestFit="1" customWidth="1"/>
@@ -1280,806 +1353,837 @@
     <col min="30" max="30" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:30" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
     <row r="3" spans="1:30" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" ht="14.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="3"/>
+      <c r="R4" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="1" t="s">
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="Z4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="AA4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="AB4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="AC4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="AD4" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="14.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="3"/>
+      <c r="Q5" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="R5" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="S5" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="T5" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="U5" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="V5" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="W5" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="X5" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="Y5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="Z5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="AA5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="AB5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="AC5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="AD5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N4" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B5" s="5" t="s">
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="3"/>
+      <c r="Q6" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="R6" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA6" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="AB6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="4"/>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="3"/>
+      <c r="Q7" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="R7" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z7" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA7" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="AB7" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7"/>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="3"/>
-      <c r="R5" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="10"/>
-      <c r="Y5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AC5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD5" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="3"/>
-      <c r="Q6" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="R6" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="S6" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="T6" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="V6" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="W6" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="X6" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="Y6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AD6" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
-      <c r="X7" s="4"/>
-      <c r="Y7" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA7" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB7" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="AC7" s="4"/>
-      <c r="AD7" s="4"/>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
+      <c r="E8" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
       <c r="N8" s="3"/>
       <c r="Q8" s="3"/>
-      <c r="R8" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="7"/>
-      <c r="Y8" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z8" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA8" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="AB8" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC8" s="7"/>
-      <c r="AD8" s="7"/>
+      <c r="R8" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA8" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC8" s="4"/>
+      <c r="AD8" s="4"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
+      <c r="A9" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
       <c r="N9" s="3"/>
       <c r="Q9" s="3"/>
-      <c r="R9" s="4" t="s">
+      <c r="R9" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA9" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="AB9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="7"/>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA10" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC10" s="4"/>
+      <c r="AD10" s="4"/>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="4"/>
-      <c r="V9" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="W9" s="4"/>
-      <c r="X9" s="4"/>
-      <c r="Y9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA9" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="AB9" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC9" s="4"/>
-      <c r="AD9" s="4"/>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="W10" s="7"/>
-      <c r="X10" s="7"/>
-      <c r="Y10" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z10" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA10" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="AB10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC10" s="7"/>
-      <c r="AD10" s="7"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="3"/>
+      <c r="B11" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="20" t="s">
+        <v>201</v>
+      </c>
       <c r="Q11" s="3"/>
-      <c r="R11" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
-      <c r="U11" s="4"/>
-      <c r="V11" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="W11" s="4"/>
-      <c r="X11" s="4"/>
-      <c r="Y11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z11" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA11" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="AB11" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC11" s="4"/>
-      <c r="AD11" s="4"/>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="6"/>
+      <c r="R11" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA11" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC11" s="6"/>
+      <c r="AD11" s="6"/>
+    </row>
+    <row r="12" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="5"/>
       <c r="N12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="S12" s="6"/>
-      <c r="T12" s="6"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="W12" s="6"/>
-      <c r="X12" s="6"/>
-      <c r="Y12" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z12" s="6" t="s">
+      <c r="R12" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB12" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC12" s="4"/>
+      <c r="AD12" s="4"/>
+    </row>
+    <row r="13" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="L13" s="6"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="3"/>
+      <c r="R13" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z13" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="AA12" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB12" s="4" t="s">
+      <c r="AA13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB13" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC13" s="6"/>
+      <c r="AD13" s="6"/>
+    </row>
+    <row r="14" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="3"/>
+      <c r="Q14" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA14" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC14" s="4"/>
+      <c r="AD14" s="4"/>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="3"/>
+      <c r="Q15" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="R15" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z15" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA15" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB15" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="AC12" s="6"/>
-      <c r="AD12" s="6"/>
-    </row>
-    <row r="13" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="I13" s="5" t="s">
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="6"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="J13" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="L13" s="4"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="W13" s="4"/>
-      <c r="X13" s="4"/>
-      <c r="Y13" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z13" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA13" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB13" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="AC13" s="4"/>
-      <c r="AD13" s="4"/>
-    </row>
-    <row r="14" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="L14" s="6"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-      <c r="V14" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="W14" s="6"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z14" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA14" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB14" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="AC14" s="6"/>
-      <c r="AD14" s="6"/>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-      <c r="U15" s="4"/>
-      <c r="V15" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="W15" s="4"/>
-      <c r="X15" s="4"/>
-      <c r="Y15" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="Z15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA15" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="AB15" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC15" s="4"/>
-      <c r="AD15" s="4"/>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="J16" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
+      <c r="I16" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
       <c r="N16" s="3"/>
       <c r="Q16" s="3"/>
-      <c r="R16" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="S16" s="6"/>
-      <c r="T16" s="6"/>
-      <c r="U16" s="6"/>
-      <c r="V16" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="W16" s="6"/>
-      <c r="X16" s="6"/>
-      <c r="Y16" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="Z16" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA16" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="AB16" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC16" s="6"/>
-      <c r="AD16" s="6"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
       <c r="N17" s="3"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="3"/>
+      <c r="Q17" s="3"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q18" s="16" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q19" s="16" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q29" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>